<commit_message>
add spares for bldg
</commit_message>
<xml_diff>
--- a/NBC_points.xlsx
+++ b/NBC_points.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipeacevedo/Documents/Programing/controller_calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EDDAD3-718D-E94D-A835-BF574EE4B395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEE8F72-AA2F-2241-B920-2A1F6F12DC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="820" windowWidth="25820" windowHeight="17440" xr2:uid="{3685C660-8D48-5847-825B-DD00EC148610}"/>
   </bookViews>
@@ -36,20 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>System</t>
   </si>
   <si>
-    <t>CHWS</t>
-  </si>
-  <si>
-    <t>HWS</t>
-  </si>
-  <si>
-    <t>AHU-1</t>
-  </si>
-  <si>
     <t>BO</t>
   </si>
   <si>
@@ -66,13 +57,58 @@
   </si>
   <si>
     <t>Pressure</t>
+  </si>
+  <si>
+    <t>UC600_test</t>
+  </si>
+  <si>
+    <t>UC600_test2</t>
+  </si>
+  <si>
+    <t>UC600_test3</t>
+  </si>
+  <si>
+    <t>UC600_test4</t>
+  </si>
+  <si>
+    <t>UC600_test5</t>
+  </si>
+  <si>
+    <t>s500test1</t>
+  </si>
+  <si>
+    <t>s500test2</t>
+  </si>
+  <si>
+    <t>s500test3</t>
+  </si>
+  <si>
+    <t>s500test4</t>
+  </si>
+  <si>
+    <t>s500test5</t>
+  </si>
+  <si>
+    <t>s500test6</t>
+  </si>
+  <si>
+    <t>s500test7</t>
+  </si>
+  <si>
+    <t>s500test8</t>
+  </si>
+  <si>
+    <t>s500test9</t>
+  </si>
+  <si>
+    <t>s500test10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,6 +120,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -460,40 +502,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E8EEC2-79BC-7246-A1C7-83C56C1C4617}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -502,36 +547,36 @@
         <v>0</v>
       </c>
       <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -539,28 +584,374 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>